<commit_message>
Added Program Edit and Delete features & step definitions
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LMS_data.xlsx
+++ b/src/test/resources/TestData/LMS_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keerthimula/git/Team4_LMSPhase2/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255F74EA-8D11-CC48-B2EC-888F3ABA145E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56226878-DAB0-0F4A-93CB-922138E8EB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{90208539-8B60-4D51-928E-C6E97A3EC16D}"/>
   </bookViews>
@@ -71,16 +71,16 @@
     <t>Active</t>
   </si>
   <si>
-    <t>SYSM00001</t>
-  </si>
-  <si>
-    <t>SM ooo345</t>
-  </si>
-  <si>
     <t>4232#</t>
   </si>
   <si>
-    <t>SM 0000078</t>
+    <t>ABC345</t>
+  </si>
+  <si>
+    <t>ABC Description</t>
+  </si>
+  <si>
+    <t>SM 000001235645</t>
   </si>
 </sst>
 </file>
@@ -584,12 +584,12 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -597,7 +597,7 @@
         <v>890364</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>